<commit_message>
database overhaul see todo.md, all projects working except SR with equalization, see announcements.md
</commit_message>
<xml_diff>
--- a/docs/expanded reproduction trial.xlsx
+++ b/docs/expanded reproduction trial.xlsx
@@ -5,15 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afree\eclipse-workspace\capitalism-8.0\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\afree\eclipse-workspace\capitalism-9.0\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10380" activeTab="1" xr2:uid="{C55A22BB-D4E7-40F3-AC2B-802623670D01}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10380" xr2:uid="{C55A22BB-D4E7-40F3-AC2B-802623670D01}"/>
   </bookViews>
   <sheets>
-    <sheet name="Balanced" sheetId="1" r:id="rId1"/>
-    <sheet name="Marx 1" sheetId="4" r:id="rId2"/>
+    <sheet name="Marx 1" sheetId="4" r:id="rId1"/>
+    <sheet name="Balanced" sheetId="1" r:id="rId2"/>
     <sheet name="constant shares of I surplus" sheetId="2" r:id="rId3"/>
     <sheet name="Marx 2" sheetId="3" r:id="rId4"/>
   </sheets>
@@ -605,244 +605,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42534A93-B2D2-4DB8-B372-B26A091E485A}">
-  <dimension ref="A2:J13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
-  <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>4000</v>
-      </c>
-      <c r="D3">
-        <v>1000</v>
-      </c>
-      <c r="E3">
-        <v>1000</v>
-      </c>
-      <c r="F3">
-        <f>SUM(C3:E3)</f>
-        <v>6000</v>
-      </c>
-      <c r="G3">
-        <f>D3/C3</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1500</v>
-      </c>
-      <c r="D4">
-        <v>750</v>
-      </c>
-      <c r="E4">
-        <v>750</v>
-      </c>
-      <c r="F4">
-        <f>SUM(C4:E4)</f>
-        <v>3000</v>
-      </c>
-      <c r="G4">
-        <f>D4/C4</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <f>SUM(C3:C4)</f>
-        <v>5500</v>
-      </c>
-      <c r="D5">
-        <f t="shared" ref="D5:E5" si="0">SUM(D3:D4)</f>
-        <v>1750</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <f>F3-C5</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A8">
-        <f>1/3</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
-        <f>C3+C6*A8</f>
-        <v>4166.666666666667</v>
-      </c>
-      <c r="D8" s="1">
-        <f>C8*G3</f>
-        <v>1041.6666666666667</v>
-      </c>
-      <c r="E8" s="1">
-        <f>D8</f>
-        <v>1041.6666666666667</v>
-      </c>
-      <c r="F8" s="1">
-        <f>SUM(C8:E8)</f>
-        <v>6250.0000000000009</v>
-      </c>
-      <c r="G8">
-        <f>D8/C8</f>
-        <v>0.25</v>
-      </c>
-      <c r="H8" s="2">
-        <f>C8-C3</f>
-        <v>166.66666666666697</v>
-      </c>
-      <c r="I8" s="2">
-        <f>D8-D3</f>
-        <v>41.666666666666742</v>
-      </c>
-      <c r="J8" s="2">
-        <f>E3-(H8+I8)</f>
-        <v>791.66666666666629</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A9">
-        <f>2/3</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1">
-        <f>C4+C6*A9</f>
-        <v>1833.3333333333333</v>
-      </c>
-      <c r="D9" s="1">
-        <f>C9*G4</f>
-        <v>916.66666666666663</v>
-      </c>
-      <c r="E9" s="1">
-        <f>D9</f>
-        <v>916.66666666666663</v>
-      </c>
-      <c r="F9" s="1">
-        <f>SUM(C9:E9)</f>
-        <v>3666.6666666666665</v>
-      </c>
-      <c r="G9">
-        <f>D9/C9</f>
-        <v>0.5</v>
-      </c>
-      <c r="H9" s="2">
-        <f>C9-C4</f>
-        <v>333.33333333333326</v>
-      </c>
-      <c r="I9" s="2">
-        <f>D9-D4</f>
-        <v>166.66666666666663</v>
-      </c>
-      <c r="J9" s="2">
-        <f>E4-(H9+I9)</f>
-        <v>250.00000000000011</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1">
-        <f>SUM(C8:C9)</f>
-        <v>6000</v>
-      </c>
-      <c r="D10" s="1">
-        <f t="shared" ref="D10" si="1">SUM(D8:D9)</f>
-        <v>1958.3333333333335</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" ref="E10" si="2">SUM(E8:E9)</f>
-        <v>1958.3333333333335</v>
-      </c>
-      <c r="J10" s="1">
-        <f>SUM(J8:J9)</f>
-        <v>1041.6666666666665</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="B11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1">
-        <f>F8-C10</f>
-        <v>250.00000000000091</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A13">
-        <f>A8</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93B651D-F4FB-4BF9-BD8B-3835EA09B3FA}">
   <dimension ref="A1:Q51"/>
   <sheetViews>
@@ -2284,6 +2046,244 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42534A93-B2D2-4DB8-B372-B26A091E485A}">
+  <dimension ref="A2:J13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="C2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="B3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>4000</v>
+      </c>
+      <c r="D3">
+        <v>1000</v>
+      </c>
+      <c r="E3">
+        <v>1000</v>
+      </c>
+      <c r="F3">
+        <f>SUM(C3:E3)</f>
+        <v>6000</v>
+      </c>
+      <c r="G3">
+        <f>D3/C3</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>1500</v>
+      </c>
+      <c r="D4">
+        <v>750</v>
+      </c>
+      <c r="E4">
+        <v>750</v>
+      </c>
+      <c r="F4">
+        <f>SUM(C4:E4)</f>
+        <v>3000</v>
+      </c>
+      <c r="G4">
+        <f>D4/C4</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <f>SUM(C3:C4)</f>
+        <v>5500</v>
+      </c>
+      <c r="D5">
+        <f t="shared" ref="D5:E5" si="0">SUM(D3:D4)</f>
+        <v>1750</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="0"/>
+        <v>1750</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6">
+        <f>F3-C5</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A8">
+        <f>1/3</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="B8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <f>C3+C6*A8</f>
+        <v>4166.666666666667</v>
+      </c>
+      <c r="D8" s="1">
+        <f>C8*G3</f>
+        <v>1041.6666666666667</v>
+      </c>
+      <c r="E8" s="1">
+        <f>D8</f>
+        <v>1041.6666666666667</v>
+      </c>
+      <c r="F8" s="1">
+        <f>SUM(C8:E8)</f>
+        <v>6250.0000000000009</v>
+      </c>
+      <c r="G8">
+        <f>D8/C8</f>
+        <v>0.25</v>
+      </c>
+      <c r="H8" s="2">
+        <f>C8-C3</f>
+        <v>166.66666666666697</v>
+      </c>
+      <c r="I8" s="2">
+        <f>D8-D3</f>
+        <v>41.666666666666742</v>
+      </c>
+      <c r="J8" s="2">
+        <f>E3-(H8+I8)</f>
+        <v>791.66666666666629</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A9">
+        <f>2/3</f>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1">
+        <f>C4+C6*A9</f>
+        <v>1833.3333333333333</v>
+      </c>
+      <c r="D9" s="1">
+        <f>C9*G4</f>
+        <v>916.66666666666663</v>
+      </c>
+      <c r="E9" s="1">
+        <f>D9</f>
+        <v>916.66666666666663</v>
+      </c>
+      <c r="F9" s="1">
+        <f>SUM(C9:E9)</f>
+        <v>3666.6666666666665</v>
+      </c>
+      <c r="G9">
+        <f>D9/C9</f>
+        <v>0.5</v>
+      </c>
+      <c r="H9" s="2">
+        <f>C9-C4</f>
+        <v>333.33333333333326</v>
+      </c>
+      <c r="I9" s="2">
+        <f>D9-D4</f>
+        <v>166.66666666666663</v>
+      </c>
+      <c r="J9" s="2">
+        <f>E4-(H9+I9)</f>
+        <v>250.00000000000011</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1">
+        <f>SUM(C8:C9)</f>
+        <v>6000</v>
+      </c>
+      <c r="D10" s="1">
+        <f t="shared" ref="D10" si="1">SUM(D8:D9)</f>
+        <v>1958.3333333333335</v>
+      </c>
+      <c r="E10" s="1">
+        <f t="shared" ref="E10" si="2">SUM(E8:E9)</f>
+        <v>1958.3333333333335</v>
+      </c>
+      <c r="J10" s="1">
+        <f>SUM(J8:J9)</f>
+        <v>1041.6666666666665</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C11" s="1">
+        <f>F8-C10</f>
+        <v>250.00000000000091</v>
+      </c>
+      <c r="D11" s="1"/>
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
+      <c r="A13">
+        <f>A8</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD7047CB-DBCC-4C79-8E88-4CF9C44E7C42}">
   <dimension ref="A1:M51"/>

</xml_diff>

<commit_message>
Working version for all four benchmark projects, user guide needs some updating
</commit_message>
<xml_diff>
--- a/docs/expanded reproduction trial.xlsx
+++ b/docs/expanded reproduction trial.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="30">
   <si>
     <t>DI</t>
   </si>
@@ -106,6 +106,18 @@
   <si>
     <t>unknown</t>
   </si>
+  <si>
+    <t>Money received</t>
+  </si>
+  <si>
+    <t>Money spent</t>
+  </si>
+  <si>
+    <t>+Accumulation funds received</t>
+  </si>
+  <si>
+    <t>-Profits repatriated</t>
+  </si>
 </sst>
 </file>
 
@@ -162,7 +174,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -178,6 +190,12 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -606,13 +624,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93B651D-F4FB-4BF9-BD8B-3835EA09B3FA}">
-  <dimension ref="A1:Q51"/>
+  <dimension ref="A1:S51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" sqref="A1:XFD1"/>
+      <selection pane="bottomRight" activeCell="T2" sqref="T1:T2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -622,9 +640,10 @@
     <col min="10" max="10" width="10.3515625" customWidth="1"/>
     <col min="11" max="13" width="11.29296875" customWidth="1"/>
     <col min="14" max="14" width="8.9375" style="3"/>
+    <col min="19" max="19" width="10.234375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
       <c r="A1" t="s">
         <v>22</v>
       </c>
@@ -632,8 +651,12 @@
         <v>0.1</v>
       </c>
       <c r="N1"/>
-    </row>
-    <row r="2" spans="1:17" ht="43" x14ac:dyDescent="0.5">
+      <c r="P1" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="Q1" s="13"/>
+    </row>
+    <row r="2" spans="1:19" ht="57.35" x14ac:dyDescent="0.5">
       <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
@@ -673,10 +696,20 @@
       <c r="O2" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="P2" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="R2" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="S2" s="12" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -723,8 +756,15 @@
         <f>E3/(C3+D3)</f>
         <v>0.2</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="P3">
+        <v>5500</v>
+      </c>
+      <c r="Q3">
+        <f>C3+D3</f>
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.5">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -771,8 +811,16 @@
         <f>E4/(C4+D4)</f>
         <v>0.33333333333333331</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.5">
+      <c r="P4">
+        <f>F4</f>
+        <v>3000</v>
+      </c>
+      <c r="Q4">
+        <f>C4+D4</f>
+        <v>2250</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.5">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -823,7 +871,7 @@
         <v>0.2413793103448276</v>
       </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.5">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -840,10 +888,10 @@
       </c>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.5">
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.5">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -893,7 +941,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.5">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -947,7 +995,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.5">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1004,7 +1052,7 @@
         <v>1.0666666666666667</v>
       </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.5">
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1023,13 +1071,13 @@
       </c>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.5">
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="7"/>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.5">
       <c r="B13" t="s">
         <v>0</v>
       </c>
@@ -1080,7 +1128,7 @@
       </c>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.5">
       <c r="B14" t="s">
         <v>1</v>
       </c>
@@ -1134,7 +1182,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.5">
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
@@ -1191,7 +1239,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.5">
       <c r="B16" s="1" t="s">
         <v>2</v>
       </c>
@@ -2037,6 +2085,9 @@
       <c r="E51" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="P1:Q1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Five benchmark projects working. New Executable
</commit_message>
<xml_diff>
--- a/docs/expanded reproduction trial.xlsx
+++ b/docs/expanded reproduction trial.xlsx
@@ -12,10 +12,11 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10380" xr2:uid="{C55A22BB-D4E7-40F3-AC2B-802623670D01}"/>
   </bookViews>
   <sheets>
-    <sheet name="Marx 1" sheetId="4" r:id="rId1"/>
-    <sheet name="Balanced" sheetId="1" r:id="rId2"/>
-    <sheet name="constant shares of I surplus" sheetId="2" r:id="rId3"/>
-    <sheet name="Marx 2" sheetId="3" r:id="rId4"/>
+    <sheet name="Simple Reproduction" sheetId="5" r:id="rId1"/>
+    <sheet name="Marx 1" sheetId="4" r:id="rId2"/>
+    <sheet name="Marx 2" sheetId="3" r:id="rId3"/>
+    <sheet name="Balanced" sheetId="1" r:id="rId4"/>
+    <sheet name="constant shares of I surplus" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="38">
   <si>
     <t>DI</t>
   </si>
@@ -117,6 +118,30 @@
   </si>
   <si>
     <t>-Profits repatriated</t>
+  </si>
+  <si>
+    <t>1 good</t>
+  </si>
+  <si>
+    <t>2 goods</t>
+  </si>
+  <si>
+    <t>DIIa</t>
+  </si>
+  <si>
+    <t>DIIb</t>
+  </si>
+  <si>
+    <t>Rate of exploitation</t>
+  </si>
+  <si>
+    <t>Capitalist Consumption</t>
+  </si>
+  <si>
+    <t>Production Split Luxuries/Total</t>
+  </si>
+  <si>
+    <t>Proportion of Luxury Consumption in Capitalist Consumption</t>
   </si>
 </sst>
 </file>
@@ -221,6 +246,117 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
+      <xdr:colOff>550334</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>46567</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>486834</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>55033</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="6" name="Straight Arrow Connector 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53C1DF64-0FCC-46D8-BF72-923178B28046}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3767667" y="2230967"/>
+          <a:ext cx="1689100" cy="8466"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>524934</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>135467</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="9" name="Straight Arrow Connector 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45A8BF71-4959-43B6-92D5-3A5CE101A516}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3742267" y="2311400"/>
+          <a:ext cx="867833" cy="8467"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>575734</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
@@ -316,6 +452,215 @@
         </a:fillRef>
         <a:effectRef idx="0">
           <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>529166</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>122767</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>406400</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>118533</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="5" name="Straight Arrow Connector 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC580F9D-B36A-4765-AB17-67B2620F350F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3103033" y="1397000"/>
+          <a:ext cx="3962400" cy="905933"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>575733</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>97367</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>402166</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>122767</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Straight Arrow Connector 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{98529F54-EE19-4BEF-ADF8-5076CBD55841}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3149600" y="1371600"/>
+          <a:ext cx="3166533" cy="25400"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>592666</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>55033</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>46567</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="10" name="Straight Connector 9">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{164B918A-1677-4BBC-99E7-BC222CB0C028}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3166533" y="2057400"/>
+          <a:ext cx="3937000" cy="901700"/>
+        </a:xfrm>
+        <a:prstGeom prst="line">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>67734</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>423333</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>105833</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="12" name="Straight Arrow Connector 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7B7CD43-7651-4E24-9757-AC39AC430F67}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3217333" y="2070101"/>
+          <a:ext cx="3119967" cy="38099"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
         </a:effectRef>
         <a:fontRef idx="minor">
           <a:schemeClr val="tx1"/>
@@ -623,14 +968,283 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECE59FE-C8CF-46B2-8E67-2ECAE9AA0094}">
+  <dimension ref="A1:H16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <cols>
+    <col min="7" max="7" width="15.41015625" customWidth="1"/>
+    <col min="8" max="8" width="14.46875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="28.7" x14ac:dyDescent="0.5">
+      <c r="C3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4">
+        <v>4000</v>
+      </c>
+      <c r="D4">
+        <f>(F4-C4)/(1+$E$1)</f>
+        <v>1000</v>
+      </c>
+      <c r="E4">
+        <f>D4*$E$1</f>
+        <v>1000</v>
+      </c>
+      <c r="F4">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B5" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>2000</v>
+      </c>
+      <c r="D5">
+        <f>(F5-C5)/(1+$E$1)</f>
+        <v>500</v>
+      </c>
+      <c r="E5">
+        <f>D5*$E$1</f>
+        <v>500</v>
+      </c>
+      <c r="F5">
+        <v>3000</v>
+      </c>
+      <c r="G5">
+        <f>D6</f>
+        <v>1500</v>
+      </c>
+      <c r="H5">
+        <f>E6</f>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B6" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6">
+        <f>SUM(C4:C5)</f>
+        <v>6000</v>
+      </c>
+      <c r="D6">
+        <f t="shared" ref="D6:H6" si="0">SUM(D4:D5)</f>
+        <v>1500</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>9000</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B9" t="s">
+        <v>36</v>
+      </c>
+      <c r="E9" s="7">
+        <f>0.2</f>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="C10" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="E10" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B11" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <v>4000</v>
+      </c>
+      <c r="D11">
+        <f>(F11-C11)/(1+$E$1)</f>
+        <v>1000</v>
+      </c>
+      <c r="E11">
+        <f>D11*$E$1</f>
+        <v>1000</v>
+      </c>
+      <c r="F11">
+        <f>F4</f>
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12">
+        <f>C5-C13</f>
+        <v>1600</v>
+      </c>
+      <c r="D12">
+        <f>(F12-C12)/(1+$E$1)</f>
+        <v>400</v>
+      </c>
+      <c r="E12">
+        <f>D12*$E$1</f>
+        <v>400</v>
+      </c>
+      <c r="F12">
+        <f>F5-F13</f>
+        <v>2400</v>
+      </c>
+      <c r="G12">
+        <f>D14</f>
+        <v>1500</v>
+      </c>
+      <c r="H12">
+        <f>F12-G12</f>
+        <v>900</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+      <c r="C13">
+        <f>C5*$E$9</f>
+        <v>400</v>
+      </c>
+      <c r="D13">
+        <f>(F13-C13)/(1+$E$1)</f>
+        <v>100</v>
+      </c>
+      <c r="E13">
+        <f>D13*$E$1</f>
+        <v>100</v>
+      </c>
+      <c r="F13">
+        <f>F5*$E$9</f>
+        <v>600</v>
+      </c>
+      <c r="H13">
+        <f>F13</f>
+        <v>600</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14">
+        <f>SUM(C11:C13)</f>
+        <v>6000</v>
+      </c>
+      <c r="D14">
+        <f t="shared" ref="D14:F14" si="1">SUM(D11:D13)</f>
+        <v>1500</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>1500</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>9000</v>
+      </c>
+      <c r="G14">
+        <f t="shared" ref="G14:H14" si="2">D14</f>
+        <v>1500</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="H16">
+        <f>H13/H14</f>
+        <v>0.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93B651D-F4FB-4BF9-BD8B-3835EA09B3FA}">
   <dimension ref="A1:S51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="T2" sqref="T1:T2"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
@@ -640,6 +1254,7 @@
     <col min="10" max="10" width="10.3515625" customWidth="1"/>
     <col min="11" max="13" width="11.29296875" customWidth="1"/>
     <col min="14" max="14" width="8.9375" style="3"/>
+    <col min="18" max="18" width="11.41015625" customWidth="1"/>
     <col min="19" max="19" width="10.234375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -656,7 +1271,7 @@
       </c>
       <c r="Q1" s="13"/>
     </row>
-    <row r="2" spans="1:19" ht="57.35" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:19" ht="43" x14ac:dyDescent="0.5">
       <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
@@ -1051,6 +1666,7 @@
         <f>F9/F4</f>
         <v>1.0666666666666667</v>
       </c>
+      <c r="R10" s="2"/>
     </row>
     <row r="11" spans="1:19" x14ac:dyDescent="0.5">
       <c r="B11" s="1" t="s">
@@ -2097,7 +2713,19 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19ACF69-7FFE-4A2A-B113-59212DF34BEC}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42534A93-B2D2-4DB8-B372-B26A091E485A}">
   <dimension ref="A2:J13"/>
   <sheetViews>
@@ -2335,7 +2963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD7047CB-DBCC-4C79-8E88-4CF9C44E7C42}">
   <dimension ref="A1:M51"/>
   <sheetViews>
@@ -3772,16 +4400,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19ACF69-7FFE-4A2A-B113-59212DF34BEC}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Data for 2 production goods incorporated, code incomplete
</commit_message>
<xml_diff>
--- a/docs/expanded reproduction trial.xlsx
+++ b/docs/expanded reproduction trial.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="10380" xr2:uid="{C55A22BB-D4E7-40F3-AC2B-802623670D01}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25602" windowHeight="10380" activeTab="1" xr2:uid="{C55A22BB-D4E7-40F3-AC2B-802623670D01}"/>
   </bookViews>
   <sheets>
     <sheet name="Simple Reproduction" sheetId="5" r:id="rId1"/>
-    <sheet name="Marx 1" sheetId="4" r:id="rId2"/>
-    <sheet name="Marx 2" sheetId="3" r:id="rId3"/>
-    <sheet name="Balanced" sheetId="1" r:id="rId4"/>
+    <sheet name="SR  with two MP" sheetId="7" r:id="rId2"/>
+    <sheet name="Marx 1" sheetId="4" r:id="rId3"/>
+    <sheet name="Marx 2" sheetId="3" r:id="rId4"/>
     <sheet name="constant shares of I surplus" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="39">
   <si>
     <t>DI</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Delta V</t>
   </si>
   <si>
-    <t>Capitalist consumptio</t>
-  </si>
-  <si>
     <t>Rate of profit</t>
   </si>
   <si>
@@ -79,9 +76,6 @@
   </si>
   <si>
     <t>Growth</t>
-  </si>
-  <si>
-    <t>TBD</t>
   </si>
   <si>
     <t>Constant share of the surplus product of I</t>
@@ -142,6 +136,15 @@
   </si>
   <si>
     <t>Proportion of Luxury Consumption in Capitalist Consumption</t>
+  </si>
+  <si>
+    <t>Fixed</t>
+  </si>
+  <si>
+    <t>Raw Materials</t>
+  </si>
+  <si>
+    <t>Consumption</t>
   </si>
 </sst>
 </file>
@@ -971,28 +974,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECE59FE-C8CF-46B2-8E67-2ECAE9AA0094}">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:H6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="7" max="7" width="15.41015625" customWidth="1"/>
-    <col min="8" max="8" width="14.46875" customWidth="1"/>
+    <col min="7" max="7" width="15.41796875" customWidth="1"/>
+    <col min="8" max="8" width="14.47265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E1" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="28.7" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="C3" s="6" t="s">
         <v>3</v>
       </c>
@@ -1006,13 +1009,13 @@
         <v>6</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="H3" s="6" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.5">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>0</v>
       </c>
@@ -1031,7 +1034,7 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
         <v>1</v>
       </c>
@@ -1058,7 +1061,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
         <v>7</v>
       </c>
@@ -1087,21 +1090,21 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.5">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E9" s="7">
         <f>0.2</f>
         <v>0.2</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="C10" s="6" t="s">
         <v>3</v>
       </c>
@@ -1117,7 +1120,7 @@
       <c r="G10" s="6"/>
       <c r="H10" s="6"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" t="s">
         <v>0</v>
       </c>
@@ -1137,9 +1140,9 @@
         <v>6000</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C12">
         <f>C5-C13</f>
@@ -1166,9 +1169,9 @@
         <v>900</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C13">
         <f>C5*$E$9</f>
@@ -1191,7 +1194,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" t="s">
         <v>7</v>
       </c>
@@ -1220,9 +1223,9 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H16">
         <f>H13/H14</f>
@@ -1237,6 +1240,173 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1C77ED3-DCBF-4325-9E6B-9BF828DE079E}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="8" max="8" width="11.3125" customWidth="1"/>
+    <col min="9" max="9" width="13.15625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+      <c r="C3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C4">
+        <v>1000</v>
+      </c>
+      <c r="D4">
+        <v>1000</v>
+      </c>
+      <c r="E4">
+        <v>500</v>
+      </c>
+      <c r="F4">
+        <v>500</v>
+      </c>
+      <c r="G4">
+        <v>3000</v>
+      </c>
+      <c r="H4">
+        <f>E4</f>
+        <v>500</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I6" si="0">F4</f>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B5" t="s">
+        <v>37</v>
+      </c>
+      <c r="C5">
+        <v>2000</v>
+      </c>
+      <c r="E5">
+        <v>500</v>
+      </c>
+      <c r="F5">
+        <f>E5*$F$1</f>
+        <v>500</v>
+      </c>
+      <c r="G5">
+        <v>3000</v>
+      </c>
+      <c r="H5">
+        <f t="shared" ref="H5:H6" si="1">E5</f>
+        <v>500</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B6" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6">
+        <v>2000</v>
+      </c>
+      <c r="E6">
+        <f>(G6-D6)/(1+$F$1)</f>
+        <v>500</v>
+      </c>
+      <c r="F6">
+        <f>E6*$F$1</f>
+        <v>500</v>
+      </c>
+      <c r="G6">
+        <v>3000</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>500</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="0"/>
+        <v>500</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <f>SUM(C4:C6)</f>
+        <v>3000</v>
+      </c>
+      <c r="D7">
+        <f>SUM(D4:D6)</f>
+        <v>3000</v>
+      </c>
+      <c r="E7">
+        <f>SUM(E4:E6)</f>
+        <v>1500</v>
+      </c>
+      <c r="F7">
+        <f>SUM(F4:F6)</f>
+        <v>1500</v>
+      </c>
+      <c r="G7">
+        <f>SUM(G4:G6)</f>
+        <v>9000</v>
+      </c>
+      <c r="H7">
+        <f>SUM(H4:H6)</f>
+        <v>1500</v>
+      </c>
+      <c r="I7">
+        <f>SUM(I4:I6)</f>
+        <v>1500</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93B651D-F4FB-4BF9-BD8B-3835EA09B3FA}">
   <dimension ref="A1:S51"/>
   <sheetViews>
@@ -1244,23 +1414,23 @@
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="B2" sqref="B2:F5"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="5" max="6" width="8.9375" customWidth="1"/>
-    <col min="7" max="7" width="10.64453125" customWidth="1"/>
-    <col min="10" max="10" width="10.3515625" customWidth="1"/>
-    <col min="11" max="13" width="11.29296875" customWidth="1"/>
-    <col min="14" max="14" width="8.9375" style="3"/>
-    <col min="18" max="18" width="11.41015625" customWidth="1"/>
-    <col min="19" max="19" width="10.234375" customWidth="1"/>
+    <col min="5" max="6" width="8.9453125" customWidth="1"/>
+    <col min="7" max="7" width="10.62890625" customWidth="1"/>
+    <col min="10" max="10" width="10.3671875" customWidth="1"/>
+    <col min="11" max="13" width="11.3125" customWidth="1"/>
+    <col min="14" max="14" width="8.9453125" style="3"/>
+    <col min="18" max="18" width="11.41796875" customWidth="1"/>
+    <col min="19" max="19" width="10.20703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C1" s="7">
         <v>0.1</v>
@@ -1271,7 +1441,7 @@
       </c>
       <c r="Q1" s="13"/>
     </row>
-    <row r="2" spans="1:19" ht="43" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="C2" s="6" t="s">
         <v>3</v>
       </c>
@@ -1285,7 +1455,7 @@
         <v>6</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="H2" s="6" t="s">
         <v>9</v>
@@ -1294,37 +1464,37 @@
         <v>10</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="L2" s="6" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="M2" s="6" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="N2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="P2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q2" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="R2" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="S2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="R2" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="S2" s="12" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.5">
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -1358,14 +1528,14 @@
         <v>500</v>
       </c>
       <c r="K3" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L3" s="2">
         <f>D3</f>
         <v>1000</v>
       </c>
       <c r="M3" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="N3" s="3">
         <f>E3/(C3+D3)</f>
@@ -1379,7 +1549,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B4" t="s">
         <v>1</v>
       </c>
@@ -1413,14 +1583,14 @@
         <v>150</v>
       </c>
       <c r="K4" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L4" s="2">
         <f>D4</f>
         <v>750</v>
       </c>
       <c r="M4" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="N4" s="3">
         <f>E4/(C4+D4)</f>
@@ -1435,7 +1605,7 @@
         <v>2250</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B5" t="s">
         <v>7</v>
       </c>
@@ -1472,21 +1642,21 @@
         <v>650</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="L5" s="2">
         <f>D5</f>
         <v>1750</v>
       </c>
       <c r="M5" s="11" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="N5" s="3">
         <f>E5/(C5+D5)</f>
         <v>0.2413793103448276</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -1495,7 +1665,7 @@
         <v>500</v>
       </c>
       <c r="F6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G6">
         <f>F4/F3</f>
@@ -1503,10 +1673,10 @@
       </c>
       <c r="H6" s="4"/>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="G7" s="10"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -1556,7 +1726,7 @@
         <v>0.2</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B9" t="s">
         <v>1</v>
       </c>
@@ -1610,7 +1780,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B10" s="1" t="s">
         <v>7</v>
       </c>
@@ -1668,7 +1838,7 @@
       </c>
       <c r="R10" s="2"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
@@ -1679,7 +1849,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
       <c r="F11" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G11" s="10">
         <f>F9/F8</f>
@@ -1687,13 +1857,13 @@
       </c>
       <c r="H11" s="4"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="7"/>
       <c r="G12" s="10"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" t="s">
         <v>0</v>
       </c>
@@ -1744,7 +1914,7 @@
       </c>
       <c r="O13" s="5"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" t="s">
         <v>1</v>
       </c>
@@ -1798,7 +1968,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="1" t="s">
         <v>7</v>
       </c>
@@ -1855,7 +2025,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="1" t="s">
         <v>2</v>
       </c>
@@ -1866,7 +2036,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
       <c r="F16" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G16" s="10">
         <f>F14/F13</f>
@@ -1874,10 +2044,10 @@
       </c>
       <c r="H16" s="4"/>
     </row>
-    <row r="17" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="17" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="G17" s="10"/>
     </row>
-    <row r="18" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="18" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" t="s">
         <v>0</v>
       </c>
@@ -1928,7 +2098,7 @@
       </c>
       <c r="O18" s="5"/>
     </row>
-    <row r="19" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="19" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" t="s">
         <v>1</v>
       </c>
@@ -1982,7 +2152,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="20" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="20" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="1" t="s">
         <v>7</v>
       </c>
@@ -2039,7 +2209,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="21" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="21" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="1" t="s">
         <v>2</v>
       </c>
@@ -2050,17 +2220,17 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
       <c r="F21" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G21" s="10">
         <f>F19/F18</f>
         <v>0.48484848484848486</v>
       </c>
     </row>
-    <row r="22" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="22" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="G22" s="10"/>
     </row>
-    <row r="23" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="23" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
         <v>0</v>
       </c>
@@ -2111,7 +2281,7 @@
       </c>
       <c r="O23" s="5"/>
     </row>
-    <row r="24" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="24" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" t="s">
         <v>1</v>
       </c>
@@ -2165,7 +2335,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="25" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="25" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" s="1" t="s">
         <v>7</v>
       </c>
@@ -2222,7 +2392,7 @@
         <v>1.0999999999999999</v>
       </c>
     </row>
-    <row r="26" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="26" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="1" t="s">
         <v>2</v>
       </c>
@@ -2233,17 +2403,17 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
       <c r="F26" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G26" s="10">
         <f>F24/F23</f>
         <v>0.48484848484848481</v>
       </c>
     </row>
-    <row r="27" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="27" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="G27" s="10"/>
     </row>
-    <row r="28" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="28" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" t="s">
         <v>0</v>
       </c>
@@ -2294,7 +2464,7 @@
       </c>
       <c r="O28" s="5"/>
     </row>
-    <row r="29" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="29" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B29" t="s">
         <v>1</v>
       </c>
@@ -2348,7 +2518,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="30" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="30" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="1" t="s">
         <v>7</v>
       </c>
@@ -2405,7 +2575,7 @@
         <v>1.1000000000000003</v>
       </c>
     </row>
-    <row r="31" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="31" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="1" t="s">
         <v>2</v>
       </c>
@@ -2416,17 +2586,17 @@
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
       <c r="F31" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G31" s="10">
         <f>F29/F28</f>
         <v>0.48484848484848486</v>
       </c>
     </row>
-    <row r="32" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="32" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="G32" s="10"/>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" t="s">
         <v>0</v>
       </c>
@@ -2462,7 +2632,7 @@
       <c r="M33" s="2"/>
       <c r="O33" s="5"/>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B34" t="s">
         <v>1</v>
       </c>
@@ -2501,7 +2671,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B35" s="1" t="s">
         <v>7</v>
       </c>
@@ -2547,7 +2717,7 @@
         <v>1.0999999999999996</v>
       </c>
     </row>
-    <row r="36" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="36" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" s="1" t="s">
         <v>2</v>
       </c>
@@ -2558,14 +2728,14 @@
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
       <c r="F36" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G36" s="10">
         <f>F34/F33</f>
         <v>0.48484848484848464</v>
       </c>
     </row>
-    <row r="38" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
@@ -2577,7 +2747,7 @@
       <c r="L38" s="2"/>
       <c r="M38" s="2"/>
     </row>
-    <row r="39" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
@@ -2590,7 +2760,7 @@
       <c r="M39" s="2"/>
       <c r="O39" s="5"/>
     </row>
-    <row r="40" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -2604,13 +2774,13 @@
       <c r="M40" s="1"/>
       <c r="O40" s="5"/>
     </row>
-    <row r="41" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="41" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" s="1"/>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="43" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="43" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
@@ -2622,7 +2792,7 @@
       <c r="L43" s="2"/>
       <c r="M43" s="2"/>
     </row>
-    <row r="44" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="44" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
@@ -2635,7 +2805,7 @@
       <c r="M44" s="2"/>
       <c r="O44" s="5"/>
     </row>
-    <row r="45" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="45" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B45" s="1"/>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
@@ -2649,13 +2819,13 @@
       <c r="M45" s="1"/>
       <c r="O45" s="5"/>
     </row>
-    <row r="46" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="46" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="48" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="C48" s="1"/>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
@@ -2667,7 +2837,7 @@
       <c r="L48" s="2"/>
       <c r="M48" s="2"/>
     </row>
-    <row r="49" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="49" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="C49" s="1"/>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
@@ -2680,7 +2850,7 @@
       <c r="M49" s="2"/>
       <c r="O49" s="5"/>
     </row>
-    <row r="50" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="50" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B50" s="1"/>
       <c r="C50" s="1"/>
       <c r="D50" s="1"/>
@@ -2694,7 +2864,7 @@
       <c r="M50" s="1"/>
       <c r="O50" s="5"/>
     </row>
-    <row r="51" spans="2:15" x14ac:dyDescent="0.5">
+    <row r="51" spans="2:15" x14ac:dyDescent="0.55000000000000004">
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
       <c r="D51" s="1"/>
@@ -2713,252 +2883,14 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D19ACF69-7FFE-4A2A-B113-59212DF34BEC}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42534A93-B2D2-4DB8-B372-B26A091E485A}">
-  <dimension ref="A2:J13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
-  <sheetData>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="C2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I2" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="B3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3">
-        <v>4000</v>
-      </c>
-      <c r="D3">
-        <v>1000</v>
-      </c>
-      <c r="E3">
-        <v>1000</v>
-      </c>
-      <c r="F3">
-        <f>SUM(C3:E3)</f>
-        <v>6000</v>
-      </c>
-      <c r="G3">
-        <f>D3/C3</f>
-        <v>0.25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4">
-        <v>1500</v>
-      </c>
-      <c r="D4">
-        <v>750</v>
-      </c>
-      <c r="E4">
-        <v>750</v>
-      </c>
-      <c r="F4">
-        <f>SUM(C4:E4)</f>
-        <v>3000</v>
-      </c>
-      <c r="G4">
-        <f>D4/C4</f>
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <f>SUM(C3:C4)</f>
-        <v>5500</v>
-      </c>
-      <c r="D5">
-        <f t="shared" ref="D5:E5" si="0">SUM(D3:D4)</f>
-        <v>1750</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="0"/>
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="B6" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6">
-        <f>F3-C5</f>
-        <v>500</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A8">
-        <f>1/3</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="B8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C8" s="1">
-        <f>C3+C6*A8</f>
-        <v>4166.666666666667</v>
-      </c>
-      <c r="D8" s="1">
-        <f>C8*G3</f>
-        <v>1041.6666666666667</v>
-      </c>
-      <c r="E8" s="1">
-        <f>D8</f>
-        <v>1041.6666666666667</v>
-      </c>
-      <c r="F8" s="1">
-        <f>SUM(C8:E8)</f>
-        <v>6250.0000000000009</v>
-      </c>
-      <c r="G8">
-        <f>D8/C8</f>
-        <v>0.25</v>
-      </c>
-      <c r="H8" s="2">
-        <f>C8-C3</f>
-        <v>166.66666666666697</v>
-      </c>
-      <c r="I8" s="2">
-        <f>D8-D3</f>
-        <v>41.666666666666742</v>
-      </c>
-      <c r="J8" s="2">
-        <f>E3-(H8+I8)</f>
-        <v>791.66666666666629</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A9">
-        <f>2/3</f>
-        <v>0.66666666666666663</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1</v>
-      </c>
-      <c r="C9" s="1">
-        <f>C4+C6*A9</f>
-        <v>1833.3333333333333</v>
-      </c>
-      <c r="D9" s="1">
-        <f>C9*G4</f>
-        <v>916.66666666666663</v>
-      </c>
-      <c r="E9" s="1">
-        <f>D9</f>
-        <v>916.66666666666663</v>
-      </c>
-      <c r="F9" s="1">
-        <f>SUM(C9:E9)</f>
-        <v>3666.6666666666665</v>
-      </c>
-      <c r="G9">
-        <f>D9/C9</f>
-        <v>0.5</v>
-      </c>
-      <c r="H9" s="2">
-        <f>C9-C4</f>
-        <v>333.33333333333326</v>
-      </c>
-      <c r="I9" s="2">
-        <f>D9-D4</f>
-        <v>166.66666666666663</v>
-      </c>
-      <c r="J9" s="2">
-        <f>E4-(H9+I9)</f>
-        <v>250.00000000000011</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1">
-        <f>SUM(C8:C9)</f>
-        <v>6000</v>
-      </c>
-      <c r="D10" s="1">
-        <f t="shared" ref="D10" si="1">SUM(D8:D9)</f>
-        <v>1958.3333333333335</v>
-      </c>
-      <c r="E10" s="1">
-        <f t="shared" ref="E10" si="2">SUM(E8:E9)</f>
-        <v>1958.3333333333335</v>
-      </c>
-      <c r="J10" s="1">
-        <f>SUM(J8:J9)</f>
-        <v>1041.6666666666665</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="B11" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C11" s="1">
-        <f>F8-C10</f>
-        <v>250.00000000000091</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.5">
-      <c r="A13">
-        <f>A8</f>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="C13" t="s">
-        <v>17</v>
-      </c>
-    </row>
-  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2974,19 +2906,19 @@
       <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="10" max="10" width="11.29296875" customWidth="1"/>
+    <col min="10" max="10" width="11.3125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="28.7" x14ac:dyDescent="0.5">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
@@ -3010,19 +2942,19 @@
         <v>10</v>
       </c>
       <c r="J2" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="K2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="L2" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="M2" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="M2" s="6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.5">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B3" t="s">
         <v>0</v>
       </c>
@@ -3044,7 +2976,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <f>C4/C3</f>
         <v>0.375</v>
@@ -3070,7 +3002,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <f>D5/C5</f>
         <v>0.31818181818181818</v>
@@ -3095,7 +3027,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -3104,7 +3036,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" t="s">
         <v>0</v>
       </c>
@@ -3141,7 +3073,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <f>C9/C8</f>
         <v>0.36363636363636365</v>
@@ -3187,7 +3119,7 @@
       </c>
       <c r="M9" s="5"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <f>D10/C10</f>
         <v>0.31666666666666665</v>
@@ -3236,7 +3168,7 @@
         <v>8.8888888888888795E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="1" t="s">
         <v>2</v>
       </c>
@@ -3247,12 +3179,12 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="7"/>
       <c r="C12" s="8"/>
       <c r="D12" s="7"/>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" t="s">
         <v>0</v>
       </c>
@@ -3289,7 +3221,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <f>C14/C13</f>
         <v>0.35245901639344263</v>
@@ -3335,7 +3267,7 @@
       </c>
       <c r="M14" s="5"/>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <f>D15/C15</f>
         <v>0.31515151515151513</v>
@@ -3384,7 +3316,7 @@
         <v>9.7959183673469452E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B16" s="1" t="s">
         <v>2</v>
       </c>
@@ -3395,7 +3327,7 @@
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B18" t="s">
         <v>0</v>
       </c>
@@ -3432,7 +3364,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <f>C19/C18</f>
         <v>0.34164222873900291</v>
@@ -3478,7 +3410,7 @@
       </c>
       <c r="M19" s="5"/>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <f>D20/C20</f>
         <v>0.31366120218579235</v>
@@ -3527,7 +3459,7 @@
         <v>0.10706319702602229</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B21" s="1" t="s">
         <v>2</v>
       </c>
@@ -3538,7 +3470,7 @@
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
         <v>0</v>
       </c>
@@ -3575,7 +3507,7 @@
         <v>500.00000000000023</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <f>C24/C23</f>
         <v>0.33133784487246232</v>
@@ -3621,7 +3553,7 @@
       </c>
       <c r="M24" s="5"/>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <f>D25/C25</f>
         <v>0.31221896383186704</v>
@@ -3670,7 +3602,7 @@
         <v>0.11605104096709207</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B26" s="1" t="s">
         <v>2</v>
       </c>
@@ -3681,7 +3613,7 @@
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B28" t="s">
         <v>0</v>
       </c>
@@ -3718,7 +3650,7 @@
         <v>500.00000000000045</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <f>C29/C28</f>
         <v>0.3216677369048711</v>
@@ -3764,7 +3696,7 @@
       </c>
       <c r="M29" s="5"/>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <f>D30/C30</f>
         <v>0.31084504598299495</v>
@@ -3813,7 +3745,7 @@
         <v>0.12478035864725001</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B31" s="1" t="s">
         <v>2</v>
       </c>
@@ -3824,7 +3756,7 @@
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B33" t="s">
         <v>0</v>
       </c>
@@ -3861,7 +3793,7 @@
         <v>500.00000000000045</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <f>C34/C33</f>
         <v>0.31271977007434054</v>
@@ -3907,7 +3839,7 @@
       </c>
       <c r="M34" s="5"/>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <f>D35/C35</f>
         <v>0.30955569825398283</v>
@@ -3956,7 +3888,7 @@
         <v>0.13312504012497617</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B36" s="1" t="s">
         <v>2</v>
       </c>
@@ -3967,7 +3899,7 @@
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" t="s">
         <v>0</v>
       </c>
@@ -4004,7 +3936,7 @@
         <v>500.00000000000045</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <f>C39/C38</f>
         <v>0.30454726987859626</v>
@@ -4050,7 +3982,7 @@
       </c>
       <c r="M39" s="5"/>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <f>D40/C40</f>
         <v>0.30836263600991209</v>
@@ -4099,7 +4031,7 @@
         <v>0.14098183562544131</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B41" s="1" t="s">
         <v>2</v>
       </c>
@@ -4110,7 +4042,7 @@
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B43" t="s">
         <v>0</v>
       </c>
@@ -4147,7 +4079,7 @@
         <v>500.00000000000182</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <f>C44/C43</f>
         <v>0.29717144042650118</v>
@@ -4193,7 +4125,7 @@
       </c>
       <c r="M44" s="5"/>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <f>D45/C45</f>
         <v>0.30727296931714615</v>
@@ -4242,7 +4174,7 @@
         <v>0.14827422967499948</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B46" s="1" t="s">
         <v>2</v>
       </c>
@@ -4253,7 +4185,7 @@
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B48" t="s">
         <v>0</v>
       </c>
@@ -4290,7 +4222,7 @@
         <v>500.00000000000227</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <f>C49/C48</f>
         <v>0.29058586276032206</v>
@@ -4336,7 +4268,7 @@
       </c>
       <c r="M49" s="5"/>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <f>D50/C50</f>
         <v>0.3062895253902001</v>
@@ -4385,7 +4317,7 @@
         <v>0.15495346931225629</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.5">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.55000000000000004">
       <c r="B51" s="1" t="s">
         <v>2</v>
       </c>

</xml_diff>

<commit_message>
profi rate equalization working
</commit_message>
<xml_diff>
--- a/docs/expanded reproduction trial.xlsx
+++ b/docs/expanded reproduction trial.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="48">
   <si>
     <t>DI</t>
   </si>
@@ -175,13 +175,25 @@
     </r>
   </si>
   <si>
-    <t>Capital</t>
+    <t>Money</t>
+  </si>
+  <si>
+    <t>Price of result</t>
+  </si>
+  <si>
+    <t>Value of result</t>
+  </si>
+  <si>
+    <t>Price-value ratio</t>
   </si>
   <si>
     <t>Price of output</t>
   </si>
   <si>
-    <t>Price/Value ratio</t>
+    <t>Capital (not including money)</t>
+  </si>
+  <si>
+    <t>Wage</t>
   </si>
 </sst>
 </file>
@@ -193,7 +205,7 @@
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="0.0%"/>
     <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;?_-;_-@_-"/>
-    <numFmt numFmtId="168" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="_-* #,##0.0000_-;\-* #,##0.0000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
@@ -268,10 +280,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -1019,10 +1031,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EECE59FE-C8CF-46B2-8E67-2ECAE9AA0094}">
-  <dimension ref="A1:M25"/>
+  <dimension ref="A1:P25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+      <selection activeCell="P25" sqref="P25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1030,8 +1042,11 @@
     <col min="1" max="1" width="19.89453125" customWidth="1"/>
     <col min="7" max="7" width="15.41796875" customWidth="1"/>
     <col min="8" max="8" width="14.47265625" customWidth="1"/>
+    <col min="9" max="9" width="12.15625" customWidth="1"/>
+    <col min="10" max="10" width="12.9453125" customWidth="1"/>
     <col min="11" max="11" width="11.15625" customWidth="1"/>
     <col min="12" max="12" width="10.7890625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.55000000000000004">
@@ -1282,7 +1297,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>39</v>
       </c>
@@ -1290,7 +1305,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" t="s">
         <v>32</v>
       </c>
@@ -1298,7 +1313,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:13" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:16" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="C22" s="6" t="s">
         <v>3</v>
       </c>
@@ -1312,26 +1327,37 @@
         <v>6</v>
       </c>
       <c r="G22" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="H22" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="I22" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="I22" s="6" t="s">
-        <v>41</v>
-      </c>
       <c r="J22" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="K22" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="K22" s="6" t="s">
+      <c r="L22" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="L22" s="6" t="s">
+      <c r="M22" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="M22" s="6"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="N22" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="O22" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="P22" s="6" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B23" t="s">
         <v>0</v>
       </c>
@@ -1349,25 +1375,39 @@
       <c r="F23">
         <v>6000</v>
       </c>
-      <c r="I23">
+      <c r="G23">
+        <v>7000</v>
+      </c>
+      <c r="J23">
         <f>C23+D23</f>
         <v>5000</v>
       </c>
-      <c r="J23" s="15">
-        <f>E23/I23</f>
+      <c r="K23" s="14">
+        <f>E23/J23</f>
         <v>0.2</v>
       </c>
-      <c r="K23" s="10">
-        <f>I23*(1+$J$25)</f>
+      <c r="L23" s="10">
+        <f>J23*(1+$K$25)</f>
         <v>6666.6666666666661</v>
       </c>
-      <c r="L23" s="15">
-        <f>K23/F23</f>
+      <c r="M23" s="1">
+        <f>J23+E23</f>
+        <v>6000</v>
+      </c>
+      <c r="N23" s="14">
+        <f>L23/M23</f>
         <v>1.1111111111111109</v>
       </c>
-      <c r="M23" s="2"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="O23" s="4">
+        <f>F23*N23</f>
+        <v>6666.6666666666661</v>
+      </c>
+      <c r="P23" s="4">
+        <f>D23*N24</f>
+        <v>888.8888888888888</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B24" t="s">
         <v>1</v>
       </c>
@@ -1385,33 +1425,47 @@
       <c r="F24" s="7">
         <v>6000</v>
       </c>
-      <c r="G24" s="7">
+      <c r="G24">
+        <v>6000</v>
+      </c>
+      <c r="H24" s="7">
         <f>D25</f>
         <v>3000</v>
       </c>
-      <c r="H24" s="7">
+      <c r="I24" s="7">
         <f>E25</f>
         <v>3000</v>
       </c>
-      <c r="I24">
-        <f t="shared" ref="I24:I25" si="3">C24+D24</f>
+      <c r="J24">
+        <f>C24+D24</f>
         <v>4000</v>
       </c>
-      <c r="J24" s="15">
-        <f t="shared" ref="J24:J25" si="4">E24/I24</f>
+      <c r="K24" s="14">
+        <f>E24/J24</f>
         <v>0.5</v>
       </c>
-      <c r="K24" s="10">
-        <f>I24*(1+$J$25)</f>
+      <c r="L24" s="10">
+        <f>J24*(1+$K$25)</f>
         <v>5333.333333333333</v>
       </c>
-      <c r="L24" s="15">
-        <f>K24/F24</f>
+      <c r="M24" s="1">
+        <f>J24+E24</f>
+        <v>6000</v>
+      </c>
+      <c r="N24" s="14">
+        <f>L24/M24</f>
         <v>0.88888888888888884</v>
       </c>
-      <c r="M24" s="2"/>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.55000000000000004">
+      <c r="O24" s="4">
+        <f>F24*N24</f>
+        <v>5333.333333333333</v>
+      </c>
+      <c r="P24" s="4">
+        <f>D24*N24</f>
+        <v>1777.7777777777776</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.55000000000000004">
       <c r="B25" t="s">
         <v>7</v>
       </c>
@@ -1420,36 +1474,56 @@
         <v>6000</v>
       </c>
       <c r="D25" s="7">
-        <f t="shared" ref="D25:H25" si="5">SUM(D23:D24)</f>
+        <f t="shared" ref="D25:G25" si="3">SUM(D23:D24)</f>
         <v>3000</v>
       </c>
       <c r="E25" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>3000</v>
       </c>
       <c r="F25" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>12000</v>
       </c>
       <c r="G25" s="7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
+        <v>13000</v>
+      </c>
+      <c r="H25" s="7">
+        <f>SUM(H23:H24)</f>
         <v>3000</v>
       </c>
-      <c r="H25" s="7">
-        <f t="shared" si="5"/>
+      <c r="I25" s="7">
+        <f>SUM(I23:I24)</f>
         <v>3000</v>
       </c>
-      <c r="I25">
-        <f t="shared" si="3"/>
+      <c r="J25">
+        <f>C25+D25</f>
         <v>9000</v>
       </c>
-      <c r="J25" s="15">
+      <c r="K25" s="14">
+        <f>E25/J25</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="L25" s="4">
+        <f>L23+L24</f>
+        <v>12000</v>
+      </c>
+      <c r="M25" s="1">
+        <f>J25+E25</f>
+        <v>12000</v>
+      </c>
+      <c r="N25" s="14">
+        <f>L25/M25</f>
+        <v>1</v>
+      </c>
+      <c r="O25" s="7">
+        <f t="shared" ref="O25:P25" si="4">SUM(O23:O24)</f>
+        <v>12000</v>
+      </c>
+      <c r="P25" s="7">
         <f t="shared" si="4"/>
-        <v>0.33333333333333331</v>
-      </c>
-      <c r="K25" s="4">
-        <f>K23+K24</f>
-        <v>12000</v>
+        <v>2666.6666666666665</v>
       </c>
     </row>
   </sheetData>
@@ -1656,10 +1730,10 @@
         <v>0.1</v>
       </c>
       <c r="N1"/>
-      <c r="P1" s="14" t="s">
+      <c r="P1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="Q1" s="14"/>
+      <c r="Q1" s="15"/>
     </row>
     <row r="2" spans="1:19" ht="43.2" x14ac:dyDescent="0.55000000000000004">
       <c r="C2" s="6" t="s">

</xml_diff>